<commit_message>
modify sending files to sending string dataframes
</commit_message>
<xml_diff>
--- a/StockerStatus_Data.xlsx
+++ b/StockerStatus_Data.xlsx
@@ -451,11 +451,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:07.975973</t>
+          <t>2022-03-15 16:59:30.279215</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>99</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3">
@@ -464,11 +464,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:09.318442</t>
+          <t>2022-03-15 16:59:35.102788</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>90</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4">
@@ -477,11 +477,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:09.946979</t>
+          <t>2022-03-15 16:59:37.241446</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>88</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5">
@@ -490,11 +490,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:10.642760</t>
+          <t>2022-03-15 16:59:38.902441</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>80</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6">
@@ -503,11 +503,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:11.242263</t>
+          <t>2022-03-15 16:59:40.005529</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>77</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7">
@@ -516,11 +516,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:12.013657</t>
+          <t>2022-03-15 16:59:41.003133</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>70</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8">
@@ -529,11 +529,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:12.648935</t>
+          <t>2022-03-15 16:59:42.059789</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>66</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9">
@@ -542,11 +542,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:13.378970</t>
+          <t>2022-03-15 16:59:43.057506</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>60</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10">
@@ -555,11 +555,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:14.129687</t>
+          <t>2022-03-15 16:59:44.279287</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>55</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11">
@@ -568,11 +568,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:14.884137</t>
+          <t>2022-03-15 16:59:45.165435</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>50</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12">
@@ -581,11 +581,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:15.625050</t>
+          <t>2022-03-15 16:59:46.874566</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>44</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13">
@@ -594,11 +594,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:16.322017</t>
+          <t>2022-03-15 16:59:50.840736</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>40</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14">
@@ -607,11 +607,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:17.036632</t>
+          <t>2022-03-15 16:59:52.000288</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>33</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15">
@@ -620,11 +620,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:19.752936</t>
+          <t>2022-03-15 16:59:53.028074</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>30</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16">
@@ -633,11 +633,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:21.448346</t>
+          <t>2022-03-15 16:59:55.712180</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>22</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17">
@@ -646,11 +646,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:22.452498</t>
+          <t>2022-03-15 16:59:57.396259</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>20</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18">
@@ -659,11 +659,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:24.037327</t>
+          <t>2022-03-15 16:59:58.823782</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>11</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19">
@@ -672,11 +672,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:25.035706</t>
+          <t>2022-03-15 17:00:00.180320</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>10</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20">
@@ -685,11 +685,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:26.080978</t>
+          <t>2022-03-15 17:00:01.755551</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>9</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21">
@@ -698,11 +698,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:26.598644</t>
+          <t>2022-03-15 17:00:03.309958</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>8</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22">
@@ -711,11 +711,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2022-03-15 15:04:27.181697</t>
+          <t>2022-03-15 17:00:04.700003</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>